<commit_message>
Fixed angle profile connector
</commit_message>
<xml_diff>
--- a/02-Rocker-Bogie-Robot/100-CHASSIS/Chassis-Dimensions.xlsx
+++ b/02-Rocker-Bogie-Robot/100-CHASSIS/Chassis-Dimensions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Chassis-Dimensions</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Rocker_Screw_Distance_Bottom</t>
+  </si>
+  <si>
+    <t>Chassis_Bottom_Height</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +508,15 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>

</xml_diff>

<commit_message>
Updated Frame of robot Updated differential
</commit_message>
<xml_diff>
--- a/02-Rocker-Bogie-Robot/100-CHASSIS/Chassis-Dimensions.xlsx
+++ b/02-Rocker-Bogie-Robot/100-CHASSIS/Chassis-Dimensions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>